<commit_message>
add labels to hw 4 datasets
</commit_message>
<xml_diff>
--- a/book/data/pcbm/wang2024_pcbm_original_experimental_data.xlsx
+++ b/book/data/pcbm/wang2024_pcbm_original_experimental_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PHD_Thesis\第2章  室内基本力学试验\paper\NC\Recised draft\二审意见\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holtw/Documents/mydocs/software/advanced-scientific-machine-learning/book/data/pcbm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B64B114-1AD7-4B8F-96A0-05998B82D294}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3B075D-5860-A24C-A8B6-7C85F533CB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13332" xr2:uid="{9FA6F14C-C309-4DBA-81DD-D5334513A472}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="13340" xr2:uid="{9FA6F14C-C309-4DBA-81DD-D5334513A472}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,16 +24,36 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>cement_percent</t>
+  </si>
+  <si>
+    <t>compaction_force_kN</t>
+  </si>
+  <si>
+    <t>compressive_strength_Mpa</t>
+  </si>
+  <si>
+    <t>porosity_percent</t>
+  </si>
+  <si>
+    <t>permeability_mms-1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.000_ "/>
+    <numFmt numFmtId="164" formatCode="0.000_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -46,7 +66,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -74,19 +94,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -102,9 +119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,7 +159,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -248,7 +265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -390,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -398,35 +415,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6DC395-D23C-4FB4-873E-0A1FF853D569}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="A1:XFD1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="8.88671875" style="2"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1">
-        <v>100</v>
-      </c>
-      <c r="C1" s="1">
-        <v>1.33</v>
-      </c>
-      <c r="D1" s="1">
-        <v>32.6</v>
-      </c>
-      <c r="E1" s="1">
-        <v>19.13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>5</v>
       </c>
@@ -434,16 +448,16 @@
         <v>100</v>
       </c>
       <c r="C2" s="1">
-        <v>1.41</v>
+        <v>1.33</v>
       </c>
       <c r="D2" s="1">
-        <v>28.51</v>
+        <v>32.6</v>
       </c>
       <c r="E2" s="1">
-        <v>20.63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19.13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>5</v>
       </c>
@@ -451,33 +465,33 @@
         <v>100</v>
       </c>
       <c r="C3" s="1">
-        <v>1.51</v>
+        <v>1.41</v>
       </c>
       <c r="D3" s="1">
-        <v>30.03</v>
+        <v>28.51</v>
       </c>
       <c r="E3" s="1">
-        <v>20.91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20.63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="C4" s="1">
-        <v>2.21</v>
+        <v>1.51</v>
       </c>
       <c r="D4" s="1">
-        <v>22.98</v>
+        <v>30.03</v>
       </c>
       <c r="E4" s="1">
-        <v>10.76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20.91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -485,16 +499,16 @@
         <v>150</v>
       </c>
       <c r="C5" s="1">
-        <v>2.25</v>
+        <v>2.21</v>
       </c>
       <c r="D5" s="1">
-        <v>28.43</v>
+        <v>22.98</v>
       </c>
       <c r="E5" s="1">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10.76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -502,33 +516,33 @@
         <v>150</v>
       </c>
       <c r="C6" s="1">
-        <v>2.4300000000000002</v>
+        <v>2.25</v>
       </c>
       <c r="D6" s="1">
-        <v>31.46</v>
+        <v>28.43</v>
       </c>
       <c r="E6" s="1">
-        <v>10.71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C7" s="1">
-        <v>3.94</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="D7" s="1">
-        <v>30.3</v>
+        <v>31.46</v>
       </c>
       <c r="E7" s="1">
-        <v>4.34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10.71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -536,16 +550,16 @@
         <v>200</v>
       </c>
       <c r="C8" s="1">
-        <v>3.78</v>
+        <v>3.94</v>
       </c>
       <c r="D8" s="1">
-        <v>22.72</v>
+        <v>30.3</v>
       </c>
       <c r="E8" s="1">
-        <v>4.16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -553,33 +567,33 @@
         <v>200</v>
       </c>
       <c r="C9" s="1">
+        <v>3.78</v>
+      </c>
+      <c r="D9" s="1">
+        <v>22.72</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>200</v>
+      </c>
+      <c r="C10" s="1">
         <v>2.97</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="1">
         <v>23.49</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="1">
         <v>5.61</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>100</v>
-      </c>
-      <c r="C10" s="1">
-        <v>3.57</v>
-      </c>
-      <c r="D10" s="1">
-        <v>26.38</v>
-      </c>
-      <c r="E10" s="1">
-        <v>8.36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -587,16 +601,16 @@
         <v>100</v>
       </c>
       <c r="C11" s="1">
-        <v>3.25</v>
+        <v>3.57</v>
       </c>
       <c r="D11" s="1">
-        <v>33.92</v>
+        <v>26.38</v>
       </c>
       <c r="E11" s="1">
-        <v>7.71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8.36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -604,33 +618,33 @@
         <v>100</v>
       </c>
       <c r="C12" s="1">
-        <v>3.28</v>
+        <v>3.25</v>
       </c>
       <c r="D12" s="1">
-        <v>29.48</v>
+        <v>33.92</v>
       </c>
       <c r="E12" s="1">
-        <v>7.52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="C13" s="1">
-        <v>5.05</v>
+        <v>3.28</v>
       </c>
       <c r="D13" s="1">
-        <v>28</v>
+        <v>29.48</v>
       </c>
       <c r="E13" s="1">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7.52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -638,16 +652,16 @@
         <v>150</v>
       </c>
       <c r="C14" s="1">
-        <v>5.53</v>
+        <v>5.05</v>
       </c>
       <c r="D14" s="1">
-        <v>21.18</v>
+        <v>28</v>
       </c>
       <c r="E14" s="1">
-        <v>3.64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -655,33 +669,33 @@
         <v>150</v>
       </c>
       <c r="C15" s="1">
-        <v>4.08</v>
+        <v>5.53</v>
       </c>
       <c r="D15" s="1">
-        <v>28.87</v>
+        <v>21.18</v>
       </c>
       <c r="E15" s="1">
-        <v>3.56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>10</v>
       </c>
       <c r="B16" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C16" s="1">
-        <v>5.62</v>
+        <v>4.08</v>
       </c>
       <c r="D16" s="1">
-        <v>23.65</v>
+        <v>28.87</v>
       </c>
       <c r="E16" s="1">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>10</v>
       </c>
@@ -689,16 +703,16 @@
         <v>200</v>
       </c>
       <c r="C17" s="1">
-        <v>7.58</v>
+        <v>5.62</v>
       </c>
       <c r="D17" s="1">
-        <v>20.27</v>
+        <v>23.65</v>
       </c>
       <c r="E17" s="1">
-        <v>1.97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>10</v>
       </c>
@@ -706,33 +720,33 @@
         <v>200</v>
       </c>
       <c r="C18" s="1">
+        <v>7.58</v>
+      </c>
+      <c r="D18" s="1">
+        <v>20.27</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1">
+        <v>200</v>
+      </c>
+      <c r="C19" s="1">
         <v>8.58</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D19" s="1">
         <v>24.71</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E19" s="1">
         <v>1.95</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1">
-        <v>100</v>
-      </c>
-      <c r="C19" s="1">
-        <v>13.82</v>
-      </c>
-      <c r="D19" s="1">
-        <v>11.26</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -740,16 +754,16 @@
         <v>100</v>
       </c>
       <c r="C20" s="1">
-        <v>15.82</v>
+        <v>13.82</v>
       </c>
       <c r="D20" s="1">
-        <v>13.96</v>
+        <v>11.26</v>
       </c>
       <c r="E20" s="1">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -757,33 +771,33 @@
         <v>100</v>
       </c>
       <c r="C21" s="1">
-        <v>12.21</v>
+        <v>15.82</v>
       </c>
       <c r="D21" s="1">
-        <v>9.01</v>
+        <v>13.96</v>
       </c>
       <c r="E21" s="1">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="C22" s="1">
-        <v>14.75</v>
+        <v>12.21</v>
       </c>
       <c r="D22" s="1">
-        <v>11.32</v>
+        <v>9.01</v>
       </c>
       <c r="E22" s="1">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -791,16 +805,16 @@
         <v>150</v>
       </c>
       <c r="C23" s="1">
-        <v>18.739999999999998</v>
+        <v>14.75</v>
       </c>
       <c r="D23" s="1">
-        <v>9.1199999999999992</v>
+        <v>11.32</v>
       </c>
       <c r="E23" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -808,33 +822,33 @@
         <v>150</v>
       </c>
       <c r="C24" s="1">
-        <v>17.55</v>
+        <v>18.739999999999998</v>
       </c>
       <c r="D24" s="1">
-        <v>11.6</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="E24" s="1">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>20</v>
       </c>
       <c r="B25" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C25" s="1">
-        <v>13.95</v>
+        <v>17.55</v>
       </c>
       <c r="D25" s="1">
-        <v>7.52</v>
+        <v>11.6</v>
       </c>
       <c r="E25" s="1">
-        <v>1.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>20</v>
       </c>
@@ -842,16 +856,16 @@
         <v>200</v>
       </c>
       <c r="C26" s="1">
-        <v>24.98</v>
+        <v>13.95</v>
       </c>
       <c r="D26" s="1">
-        <v>8.6199999999999992</v>
+        <v>7.52</v>
       </c>
       <c r="E26" s="1">
-        <v>8.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>20</v>
       </c>
@@ -859,12 +873,29 @@
         <v>200</v>
       </c>
       <c r="C27" s="1">
+        <v>24.98</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="E27" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1">
+        <v>200</v>
+      </c>
+      <c r="C28" s="1">
         <v>18.91</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D28" s="1">
         <v>11.99</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E28" s="1">
         <v>1.2E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix typo in header
</commit_message>
<xml_diff>
--- a/book/data/pcbm/wang2024_pcbm_original_experimental_data.xlsx
+++ b/book/data/pcbm/wang2024_pcbm_original_experimental_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holtw/Documents/mydocs/software/advanced-scientific-machine-learning/book/data/pcbm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3B075D-5860-A24C-A8B6-7C85F533CB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71976FD9-7C3C-F941-B4D4-4910A45BABAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="13340" xr2:uid="{9FA6F14C-C309-4DBA-81DD-D5334513A472}"/>
   </bookViews>
@@ -33,13 +33,13 @@
     <t>compaction_force_kN</t>
   </si>
   <si>
-    <t>compressive_strength_Mpa</t>
-  </si>
-  <si>
     <t>porosity_percent</t>
   </si>
   <si>
     <t>permeability_mms-1</t>
+  </si>
+  <si>
+    <t>compressive_strength_MPa</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -431,13 +431,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>